<commit_message>
Finalizing the test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/Google.xlsx
+++ b/src/test/resources/TestDataFiles/Google.xlsx
@@ -2554,7 +2554,7 @@
   <dimension ref="A1:AMJ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4631,26 +4631,26 @@
     </row>
     <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>